<commit_message>
Adapt the script to deal with fuel moisture
</commit_message>
<xml_diff>
--- a/raw_data/GroundTruth_FuelTypes05_Labeled.xlsx
+++ b/raw_data/GroundTruth_FuelTypes05_Labeled.xlsx
@@ -246,7 +246,7 @@
   <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -631,7 +631,7 @@
   </sheetPr>
   <dimension ref="A1:I212"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A178" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
@@ -5339,8 +5339,8 @@
   </sheetPr>
   <dimension ref="A1:I73"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M32" activeCellId="0" sqref="M32"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A40" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E83" activeCellId="0" sqref="E83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>